<commit_message>
modify the result file
</commit_message>
<xml_diff>
--- a/result/result_20140325.xlsx
+++ b/result/result_20140325.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="220" windowWidth="31260" windowHeight="15480" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GMM" sheetId="1" r:id="rId1"/>
@@ -331,8 +331,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="187">
+  <cellStyleXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -525,7 +529,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="187">
+  <cellStyles count="191">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="已瀏覽過的超連結" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="4" builtinId="9" hidden="1"/>
@@ -620,6 +624,8 @@
     <cellStyle name="已瀏覽過的超連結" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="190" builtinId="9" hidden="1"/>
     <cellStyle name="超連結" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="5" builtinId="8" hidden="1"/>
@@ -713,6 +719,8 @@
     <cellStyle name="超連結" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="189" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1044,7 +1052,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I27"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1136,7 +1144,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C29" si="0">E3/30</f>
+        <f t="shared" ref="C3:C20" si="0">E3/30</f>
         <v>73.766666666666666</v>
       </c>
       <c r="D3" s="1">
@@ -1146,18 +1154,18 @@
         <v>2213</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F29" si="1">D3/E3*100</f>
+        <f t="shared" ref="F3:F20" si="1">D3/E3*100</f>
         <v>28.874830546769093</v>
       </c>
       <c r="G3" s="1">
         <v>809</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H29" si="2">D3/G3*100</f>
+        <f t="shared" ref="H3:H20" si="2">D3/G3*100</f>
         <v>78.986402966625462</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I29" si="3">2*F3*H3/(F3+H3)</f>
+        <f t="shared" ref="I3:I20" si="3">2*F3*H3/(F3+H3)</f>
         <v>42.289874255459964</v>
       </c>
       <c r="J3" s="1">
@@ -1167,7 +1175,7 @@
         <v>7</v>
       </c>
       <c r="L3" s="2">
-        <f t="shared" ref="L3:L29" si="4">J3/K3*100</f>
+        <f t="shared" ref="L3:L20" si="4">J3/K3*100</f>
         <v>85.714285714285708</v>
       </c>
     </row>
@@ -1869,12 +1877,14 @@
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="B21" t="s">
         <v>39</v>
       </c>
       <c r="C21" s="1">
-        <f>E21/30</f>
+        <f t="shared" ref="C21:C27" si="5">E21/30</f>
         <v>139.5</v>
       </c>
       <c r="D21" s="1">
@@ -1884,18 +1894,18 @@
         <v>4185</v>
       </c>
       <c r="F21" s="2">
-        <f>D21/E21*100</f>
+        <f t="shared" ref="F21:F27" si="6">D21/E21*100</f>
         <v>46.953405017921149</v>
       </c>
       <c r="G21" s="1">
         <v>2341</v>
       </c>
       <c r="H21" s="2">
-        <f>D21/G21*100</f>
+        <f t="shared" ref="H21:H27" si="7">D21/G21*100</f>
         <v>83.938487825715498</v>
       </c>
       <c r="I21" s="2">
-        <f>2*F21*H21/(F21+H21)</f>
+        <f t="shared" ref="I21:I27" si="8">2*F21*H21/(F21+H21)</f>
         <v>60.220655838185721</v>
       </c>
       <c r="J21" s="1">
@@ -1905,19 +1915,16 @@
         <v>25</v>
       </c>
       <c r="L21" s="2">
-        <f>J21/K21*100</f>
+        <f t="shared" ref="L21:L27" si="9">J21/K21*100</f>
         <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="B22" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="1">
-        <f>E22/30</f>
+        <f t="shared" si="5"/>
         <v>149.73333333333332</v>
       </c>
       <c r="D22" s="1">
@@ -1927,18 +1934,18 @@
         <v>4492</v>
       </c>
       <c r="F22" s="2">
-        <f>D22/E22*100</f>
+        <f t="shared" si="6"/>
         <v>42.69813000890472</v>
       </c>
       <c r="G22" s="1">
         <v>2274</v>
       </c>
       <c r="H22" s="2">
-        <f>D22/G22*100</f>
+        <f t="shared" si="7"/>
         <v>84.344766930518915</v>
       </c>
       <c r="I22" s="2">
-        <f>2*F22*H22/(F22+H22)</f>
+        <f t="shared" si="8"/>
         <v>56.695240910434528</v>
       </c>
       <c r="J22" s="1">
@@ -1948,7 +1955,7 @@
         <v>20</v>
       </c>
       <c r="L22" s="2">
-        <f>J22/K22*100</f>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
     </row>
@@ -1958,7 +1965,7 @@
         <v>41</v>
       </c>
       <c r="C23" s="1">
-        <f>E23/30</f>
+        <f t="shared" si="5"/>
         <v>177.36666666666667</v>
       </c>
       <c r="D23" s="1">
@@ -1968,18 +1975,18 @@
         <v>5321</v>
       </c>
       <c r="F23" s="2">
-        <f>D23/E23*100</f>
+        <f t="shared" si="6"/>
         <v>31.159556474346928</v>
       </c>
       <c r="G23" s="1">
         <v>1683</v>
       </c>
       <c r="H23" s="2">
-        <f>D23/G23*100</f>
+        <f t="shared" si="7"/>
         <v>98.514557338086746</v>
       </c>
       <c r="I23" s="2">
-        <f>2*F23*H23/(F23+H23)</f>
+        <f t="shared" si="8"/>
         <v>47.344374643061101</v>
       </c>
       <c r="J23" s="1">
@@ -1989,7 +1996,7 @@
         <v>21</v>
       </c>
       <c r="L23" s="2">
-        <f>J23/K23*100</f>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
     </row>
@@ -1999,7 +2006,7 @@
         <v>42</v>
       </c>
       <c r="C24" s="1">
-        <f>E24/30</f>
+        <f t="shared" si="5"/>
         <v>67.2</v>
       </c>
       <c r="D24" s="1">
@@ -2009,18 +2016,18 @@
         <v>2016</v>
       </c>
       <c r="F24" s="2">
-        <f>D24/E24*100</f>
+        <f t="shared" si="6"/>
         <v>34.176587301587304</v>
       </c>
       <c r="G24" s="1">
         <v>854</v>
       </c>
       <c r="H24" s="2">
-        <f>D24/G24*100</f>
+        <f t="shared" si="7"/>
         <v>80.679156908665107</v>
       </c>
       <c r="I24" s="2">
-        <f>2*F24*H24/(F24+H24)</f>
+        <f t="shared" si="8"/>
         <v>48.013937282229968</v>
       </c>
       <c r="J24" s="1">
@@ -2030,17 +2037,19 @@
         <v>16</v>
       </c>
       <c r="L24" s="2">
-        <f>J24/K24*100</f>
+        <f t="shared" si="9"/>
         <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="2"/>
+      <c r="A25" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="B25" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="1">
-        <f>E25/30</f>
+        <f t="shared" si="5"/>
         <v>300.23333333333335</v>
       </c>
       <c r="D25" s="1">
@@ -2050,18 +2059,18 @@
         <v>9007</v>
       </c>
       <c r="F25" s="2">
-        <f>D25/E25*100</f>
+        <f t="shared" si="6"/>
         <v>65.282558010436333</v>
       </c>
       <c r="G25" s="1">
         <v>6522</v>
       </c>
       <c r="H25" s="2">
-        <f>D25/G25*100</f>
+        <f t="shared" si="7"/>
         <v>90.156393744250224</v>
       </c>
       <c r="I25" s="2">
-        <f>2*F25*H25/(F25+H25)</f>
+        <f t="shared" si="8"/>
         <v>75.729280700624628</v>
       </c>
       <c r="J25" s="1">
@@ -2071,19 +2080,16 @@
         <v>32</v>
       </c>
       <c r="L25" s="2">
-        <f>J25/K25*100</f>
+        <f t="shared" si="9"/>
         <v>96.875</v>
       </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="B26" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="1">
-        <f>E26/30</f>
+        <f t="shared" si="5"/>
         <v>303.33333333333331</v>
       </c>
       <c r="D26" s="1">
@@ -2093,18 +2099,18 @@
         <v>9100</v>
       </c>
       <c r="F26" s="2">
-        <f>D26/E26*100</f>
+        <f t="shared" si="6"/>
         <v>70</v>
       </c>
       <c r="G26" s="1">
         <v>6940</v>
       </c>
       <c r="H26" s="2">
-        <f>D26/G26*100</f>
+        <f t="shared" si="7"/>
         <v>91.786743515850148</v>
       </c>
       <c r="I26" s="2">
-        <f>2*F26*H26/(F26+H26)</f>
+        <f t="shared" si="8"/>
         <v>79.426433915211973</v>
       </c>
       <c r="J26" s="1">
@@ -2114,7 +2120,7 @@
         <v>33</v>
       </c>
       <c r="L26" s="2">
-        <f>J26/K26*100</f>
+        <f t="shared" si="9"/>
         <v>96.969696969696969</v>
       </c>
     </row>
@@ -2124,7 +2130,7 @@
         <v>44</v>
       </c>
       <c r="C27" s="1">
-        <f>E27/30</f>
+        <f t="shared" si="5"/>
         <v>289.7</v>
       </c>
       <c r="D27" s="1">
@@ -2134,18 +2140,18 @@
         <v>8691</v>
       </c>
       <c r="F27" s="2">
-        <f>D27/E27*100</f>
+        <f t="shared" si="6"/>
         <v>76.044183638246466</v>
       </c>
       <c r="G27" s="1">
         <v>7092</v>
       </c>
       <c r="H27" s="2">
-        <f>D27/G27*100</f>
+        <f t="shared" si="7"/>
         <v>93.189509306260575</v>
       </c>
       <c r="I27" s="2">
-        <f>2*F27*H27/(F27+H27)</f>
+        <f t="shared" si="8"/>
         <v>83.748336818095424</v>
       </c>
       <c r="J27" s="1">
@@ -2155,7 +2161,7 @@
         <v>32</v>
       </c>
       <c r="L27" s="2">
-        <f>J27/K27*100</f>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
     </row>
@@ -2253,11 +2259,11 @@
         <v>710</v>
       </c>
       <c r="I2" s="2">
-        <f>D2/H2*100</f>
+        <f t="shared" ref="I2:I27" si="0">D2/H2*100</f>
         <v>91.126760563380287</v>
       </c>
       <c r="J2" s="2">
-        <f>2*F2*I2/(F2+I2)</f>
+        <f t="shared" ref="J2:J27" si="1">2*F2*I2/(F2+I2)</f>
         <v>17.922437673130194</v>
       </c>
       <c r="K2">
@@ -2267,7 +2273,7 @@
         <v>8</v>
       </c>
       <c r="M2" s="2">
-        <f>K2/L2*100</f>
+        <f t="shared" ref="M2:M27" si="2">K2/L2*100</f>
         <v>87.5</v>
       </c>
     </row>
@@ -2276,7 +2282,7 @@
         <v>13</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C20" si="0">E3/30</f>
+        <f t="shared" ref="C3:C20" si="3">E3/30</f>
         <v>274</v>
       </c>
       <c r="D3">
@@ -2286,22 +2292,22 @@
         <v>8220</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F20" si="1">D3/E3*100</f>
+        <f t="shared" ref="F3:F20" si="4">D3/E3*100</f>
         <v>8.2481751824817504</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G27" si="2">D3</f>
+        <f t="shared" ref="G3:G27" si="5">D3</f>
         <v>678</v>
       </c>
       <c r="H3">
         <v>809</v>
       </c>
       <c r="I3" s="2">
-        <f>D3/H3*100</f>
+        <f t="shared" si="0"/>
         <v>83.807169344870218</v>
       </c>
       <c r="J3" s="2">
-        <f>2*F3*I3/(F3+I3)</f>
+        <f t="shared" si="1"/>
         <v>15.018274448997673</v>
       </c>
       <c r="K3">
@@ -2311,7 +2317,7 @@
         <v>7</v>
       </c>
       <c r="M3" s="2">
-        <f>K3/L3*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -2320,7 +2326,7 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>164</v>
       </c>
       <c r="D4">
@@ -2330,22 +2336,22 @@
         <v>4920</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>44.552845528455286</v>
       </c>
       <c r="G4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2192</v>
       </c>
       <c r="H4">
         <v>3873</v>
       </c>
       <c r="I4" s="2">
-        <f>D4/H4*100</f>
+        <f t="shared" si="0"/>
         <v>56.596953266201908</v>
       </c>
       <c r="J4" s="2">
-        <f>2*F4*I4/(F4+I4)</f>
+        <f t="shared" si="1"/>
         <v>49.857841464801552</v>
       </c>
       <c r="K4">
@@ -2355,7 +2361,7 @@
         <v>20</v>
       </c>
       <c r="M4" s="2">
-        <f>K4/L4*100</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
     </row>
@@ -2364,7 +2370,7 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>206</v>
       </c>
       <c r="D5">
@@ -2374,22 +2380,22 @@
         <v>6180</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2.2006472491909386</v>
       </c>
       <c r="G5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>136</v>
       </c>
       <c r="H5">
         <v>136</v>
       </c>
       <c r="I5" s="2">
-        <f>D5/H5*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J5" s="2">
-        <f>2*F5*I5/(F5+I5)</f>
+        <f t="shared" si="1"/>
         <v>4.3065231158961375</v>
       </c>
       <c r="K5">
@@ -2399,7 +2405,7 @@
         <v>2</v>
       </c>
       <c r="M5" s="2">
-        <f>K5/L5*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -2408,7 +2414,7 @@
         <v>16</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>153</v>
       </c>
       <c r="D6">
@@ -2418,22 +2424,22 @@
         <v>4590</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>30.152505446623096</v>
       </c>
       <c r="G6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1384</v>
       </c>
       <c r="H6">
         <v>1783</v>
       </c>
       <c r="I6" s="2">
-        <f>D6/H6*100</f>
+        <f t="shared" si="0"/>
         <v>77.621985417835106</v>
       </c>
       <c r="J6" s="2">
-        <f>2*F6*I6/(F6+I6)</f>
+        <f t="shared" si="1"/>
         <v>43.433233955750822</v>
       </c>
       <c r="K6">
@@ -2443,7 +2449,7 @@
         <v>13</v>
       </c>
       <c r="M6" s="2">
-        <f>K6/L6*100</f>
+        <f t="shared" si="2"/>
         <v>84.615384615384613</v>
       </c>
     </row>
@@ -2452,7 +2458,7 @@
         <v>17</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>274</v>
       </c>
       <c r="D7">
@@ -2462,22 +2468,22 @@
         <v>8220</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.766423357664233</v>
       </c>
       <c r="G7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>474</v>
       </c>
       <c r="H7">
         <v>505</v>
       </c>
       <c r="I7" s="2">
-        <f>D7/H7*100</f>
+        <f t="shared" si="0"/>
         <v>93.861386138613852</v>
       </c>
       <c r="J7" s="2">
-        <f>2*F7*I7/(F7+I7)</f>
+        <f t="shared" si="1"/>
         <v>10.865329512893981</v>
       </c>
       <c r="K7">
@@ -2487,7 +2493,7 @@
         <v>6</v>
       </c>
       <c r="M7" s="2">
-        <f>K7/L7*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -2496,7 +2502,7 @@
         <v>18</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>334</v>
       </c>
       <c r="D8">
@@ -2506,22 +2512,22 @@
         <v>10020</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.12974051896207586</v>
       </c>
       <c r="G8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="H8">
         <v>13</v>
       </c>
       <c r="I8" s="2">
-        <f>D8/H8*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J8" s="2">
-        <f>2*F8*I8/(F8+I8)</f>
+        <f t="shared" si="1"/>
         <v>0.25914482208711254</v>
       </c>
       <c r="K8">
@@ -2531,7 +2537,7 @@
         <v>1</v>
       </c>
       <c r="M8" s="2">
-        <f>K8/L8*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -2540,7 +2546,7 @@
         <v>19</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>327</v>
       </c>
       <c r="D9">
@@ -2550,22 +2556,22 @@
         <v>9810</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>8.3282364933741082</v>
       </c>
       <c r="G9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>817</v>
       </c>
       <c r="H9">
         <v>1203</v>
       </c>
       <c r="I9" s="2">
-        <f>D9/H9*100</f>
+        <f t="shared" si="0"/>
         <v>67.91354945968412</v>
       </c>
       <c r="J9" s="2">
-        <f>2*F9*I9/(F9+I9)</f>
+        <f t="shared" si="1"/>
         <v>14.837010805411788</v>
       </c>
       <c r="K9">
@@ -2575,7 +2581,7 @@
         <v>3</v>
       </c>
       <c r="M9" s="2">
-        <f>K9/L9*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -2584,7 +2590,7 @@
         <v>20</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>334</v>
       </c>
       <c r="D10">
@@ -2594,22 +2600,22 @@
         <v>10020</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.9860279441117765</v>
       </c>
       <c r="G10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>199</v>
       </c>
       <c r="H10">
         <v>199</v>
       </c>
       <c r="I10" s="2">
-        <f>D10/H10*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J10" s="2">
-        <f>2*F10*I10/(F10+I10)</f>
+        <f t="shared" si="1"/>
         <v>3.894705939915843</v>
       </c>
       <c r="K10">
@@ -2619,7 +2625,7 @@
         <v>2</v>
       </c>
       <c r="M10" s="2">
-        <f>K10/L10*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -2628,7 +2634,7 @@
         <v>21</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>353</v>
       </c>
       <c r="D11">
@@ -2638,22 +2644,22 @@
         <v>10590</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>8.9518413597733719</v>
       </c>
       <c r="G11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>948</v>
       </c>
       <c r="H11">
         <v>1913</v>
       </c>
       <c r="I11" s="2">
-        <f>D11/H11*100</f>
+        <f t="shared" si="0"/>
         <v>49.555671719811812</v>
       </c>
       <c r="J11" s="2">
-        <f>2*F11*I11/(F11+I11)</f>
+        <f t="shared" si="1"/>
         <v>15.164360553467171</v>
       </c>
       <c r="K11">
@@ -2663,7 +2669,7 @@
         <v>2</v>
       </c>
       <c r="M11" s="2">
-        <f>K11/L11*100</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
     </row>
@@ -2672,7 +2678,7 @@
         <v>22</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>252</v>
       </c>
       <c r="D12">
@@ -2682,22 +2688,22 @@
         <v>7560</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>18.664021164021165</v>
       </c>
       <c r="G12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1411</v>
       </c>
       <c r="H12">
         <v>2608</v>
       </c>
       <c r="I12" s="2">
-        <f>D12/H12*100</f>
+        <f t="shared" si="0"/>
         <v>54.102760736196323</v>
       </c>
       <c r="J12" s="2">
-        <f>2*F12*I12/(F12+I12)</f>
+        <f t="shared" si="1"/>
         <v>27.753737214791503</v>
       </c>
       <c r="K12">
@@ -2707,7 +2713,7 @@
         <v>3</v>
       </c>
       <c r="M12" s="2">
-        <f>K12/L12*100</f>
+        <f t="shared" si="2"/>
         <v>33.333333333333329</v>
       </c>
     </row>
@@ -2716,7 +2722,7 @@
         <v>23</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>135</v>
       </c>
       <c r="D13">
@@ -2726,22 +2732,22 @@
         <v>4050</v>
       </c>
       <c r="F13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>56.296296296296298</v>
       </c>
       <c r="G13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2280</v>
       </c>
       <c r="H13">
         <v>8142</v>
       </c>
       <c r="I13" s="2">
-        <f>D13/H13*100</f>
+        <f t="shared" si="0"/>
         <v>28.002947678703023</v>
       </c>
       <c r="J13" s="2">
-        <f>2*F13*I13/(F13+I13)</f>
+        <f t="shared" si="1"/>
         <v>37.401574803149614</v>
       </c>
       <c r="K13">
@@ -2751,7 +2757,7 @@
         <v>13</v>
       </c>
       <c r="M13" s="2">
-        <f>K13/L13*100</f>
+        <f t="shared" si="2"/>
         <v>38.461538461538467</v>
       </c>
     </row>
@@ -2760,7 +2766,7 @@
         <v>24</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>222</v>
       </c>
       <c r="D14">
@@ -2770,22 +2776,22 @@
         <v>6660</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>44.099099099099099</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2937</v>
       </c>
       <c r="H14">
         <v>4532</v>
       </c>
       <c r="I14" s="2">
-        <f>D14/H14*100</f>
+        <f t="shared" si="0"/>
         <v>64.805825242718456</v>
       </c>
       <c r="J14" s="2">
-        <f>2*F14*I14/(F14+I14)</f>
+        <f t="shared" si="1"/>
         <v>52.483917083631177</v>
       </c>
       <c r="K14">
@@ -2795,7 +2801,7 @@
         <v>16</v>
       </c>
       <c r="M14" s="2">
-        <f>K14/L14*100</f>
+        <f t="shared" si="2"/>
         <v>87.5</v>
       </c>
     </row>
@@ -2804,7 +2810,7 @@
         <v>25</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>346</v>
       </c>
       <c r="D15">
@@ -2814,22 +2820,22 @@
         <v>10380</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15" s="2" t="e">
-        <f>D15/H15*100</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J15" s="2" t="e">
-        <f>2*F15*I15/(F15+I15)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K15">
@@ -2839,7 +2845,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="2" t="e">
-        <f>K15/L15*100</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2848,7 +2854,7 @@
         <v>26</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>156</v>
       </c>
       <c r="D16">
@@ -2858,22 +2864,22 @@
         <v>4680</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>24.82905982905983</v>
       </c>
       <c r="G16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1162</v>
       </c>
       <c r="H16">
         <v>1718</v>
       </c>
       <c r="I16" s="2">
-        <f>D16/H16*100</f>
+        <f t="shared" si="0"/>
         <v>67.63678696158324</v>
       </c>
       <c r="J16" s="2">
-        <f>2*F16*I16/(F16+I16)</f>
+        <f t="shared" si="1"/>
         <v>36.3238512035011</v>
       </c>
       <c r="K16">
@@ -2883,7 +2889,7 @@
         <v>10</v>
       </c>
       <c r="M16" s="2">
-        <f>K16/L16*100</f>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
     </row>
@@ -2892,7 +2898,7 @@
         <v>27</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>157</v>
       </c>
       <c r="D17">
@@ -2902,22 +2908,22 @@
         <v>4710</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>25.35031847133758</v>
       </c>
       <c r="G17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1194</v>
       </c>
       <c r="H17">
         <v>1978</v>
       </c>
       <c r="I17" s="2">
-        <f>D17/H17*100</f>
+        <f t="shared" si="0"/>
         <v>60.364004044489384</v>
       </c>
       <c r="J17" s="2">
-        <f>2*F17*I17/(F17+I17)</f>
+        <f t="shared" si="1"/>
         <v>35.705741626794264</v>
       </c>
       <c r="K17">
@@ -2927,7 +2933,7 @@
         <v>9</v>
       </c>
       <c r="M17" s="2">
-        <f>K17/L17*100</f>
+        <f t="shared" si="2"/>
         <v>44.444444444444443</v>
       </c>
     </row>
@@ -2936,7 +2942,7 @@
         <v>28</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>154</v>
       </c>
       <c r="D18">
@@ -2946,22 +2952,22 @@
         <v>4620</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>32.640692640692642</v>
       </c>
       <c r="G18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1508</v>
       </c>
       <c r="H18">
         <v>1778</v>
       </c>
       <c r="I18" s="2">
-        <f>D18/H18*100</f>
+        <f t="shared" si="0"/>
         <v>84.814398200224971</v>
       </c>
       <c r="J18" s="2">
-        <f>2*F18*I18/(F18+I18)</f>
+        <f t="shared" si="1"/>
         <v>47.139731165989367</v>
       </c>
       <c r="K18">
@@ -2971,7 +2977,7 @@
         <v>14</v>
       </c>
       <c r="M18" s="2">
-        <f>K18/L18*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -2980,7 +2986,7 @@
         <v>29</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>167</v>
       </c>
       <c r="D19">
@@ -2990,22 +2996,22 @@
         <v>5010</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>42.355289421157686</v>
       </c>
       <c r="G19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2122</v>
       </c>
       <c r="H19">
         <v>3103</v>
       </c>
       <c r="I19" s="2">
-        <f>D19/H19*100</f>
+        <f t="shared" si="0"/>
         <v>68.385433451498542</v>
       </c>
       <c r="J19" s="2">
-        <f>2*F19*I19/(F19+I19)</f>
+        <f t="shared" si="1"/>
         <v>52.311105632934797</v>
       </c>
       <c r="K19">
@@ -3015,7 +3021,7 @@
         <v>14</v>
       </c>
       <c r="M19" s="2">
-        <f>K19/L19*100</f>
+        <f t="shared" si="2"/>
         <v>78.571428571428569</v>
       </c>
     </row>
@@ -3024,7 +3030,7 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>165</v>
       </c>
       <c r="D20">
@@ -3034,22 +3040,22 @@
         <v>4950</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>8.4848484848484862</v>
       </c>
       <c r="G20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>420</v>
       </c>
       <c r="H20">
         <v>463</v>
       </c>
       <c r="I20" s="2">
-        <f>D20/H20*100</f>
+        <f t="shared" si="0"/>
         <v>90.712742980561558</v>
       </c>
       <c r="J20" s="2">
-        <f>2*F20*I20/(F20+I20)</f>
+        <f t="shared" si="1"/>
         <v>15.518196933308703</v>
       </c>
       <c r="K20">
@@ -3059,7 +3065,7 @@
         <v>4</v>
       </c>
       <c r="M20" s="2">
-        <f>K20/L20*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -3071,7 +3077,7 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <f>E21/30</f>
+        <f t="shared" ref="C21:C27" si="6">E21/30</f>
         <v>396</v>
       </c>
       <c r="D21">
@@ -3081,22 +3087,22 @@
         <v>11880</v>
       </c>
       <c r="F21" s="2">
-        <f>D21/E21*100</f>
+        <f t="shared" ref="F21:F27" si="7">D21/E21*100</f>
         <v>15.723905723905723</v>
       </c>
       <c r="G21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1868</v>
       </c>
       <c r="H21">
         <v>2314</v>
       </c>
       <c r="I21" s="2">
-        <f>D21/H21*100</f>
+        <f t="shared" si="0"/>
         <v>80.726015557476231</v>
       </c>
       <c r="J21" s="2">
-        <f>2*F21*I21/(F21+I21)</f>
+        <f t="shared" si="1"/>
         <v>26.320980696068759</v>
       </c>
       <c r="K21">
@@ -3106,7 +3112,7 @@
         <v>25</v>
       </c>
       <c r="M21" s="2">
-        <f>K21/L21*100</f>
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
     </row>
@@ -3115,7 +3121,7 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <f>E22/30</f>
+        <f t="shared" si="6"/>
         <v>175</v>
       </c>
       <c r="D22">
@@ -3125,22 +3131,22 @@
         <v>5250</v>
       </c>
       <c r="F22" s="2">
-        <f>D22/E22*100</f>
+        <f t="shared" si="7"/>
         <v>31.752380952380953</v>
       </c>
       <c r="G22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1667</v>
       </c>
       <c r="H22">
         <v>2383</v>
       </c>
       <c r="I22" s="2">
-        <f>D22/H22*100</f>
+        <f t="shared" si="0"/>
         <v>69.953839697859848</v>
       </c>
       <c r="J22" s="2">
-        <f>2*F22*I22/(F22+I22)</f>
+        <f t="shared" si="1"/>
         <v>43.678763264771398</v>
       </c>
       <c r="K22">
@@ -3150,7 +3156,7 @@
         <v>20</v>
       </c>
       <c r="M22" s="2">
-        <f>K22/L22*100</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
     </row>
@@ -3159,7 +3165,7 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <f>E23/30</f>
+        <f t="shared" si="6"/>
         <v>275</v>
       </c>
       <c r="D23">
@@ -3169,22 +3175,22 @@
         <v>8250</v>
       </c>
       <c r="F23" s="2">
-        <f>D23/E23*100</f>
+        <f t="shared" si="7"/>
         <v>16.33939393939394</v>
       </c>
       <c r="G23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1348</v>
       </c>
       <c r="H23">
         <v>1683</v>
       </c>
       <c r="I23" s="2">
-        <f>D23/H23*100</f>
+        <f t="shared" si="0"/>
         <v>80.095068330362452</v>
       </c>
       <c r="J23" s="2">
-        <f>2*F23*I23/(F23+I23)</f>
+        <f t="shared" si="1"/>
         <v>27.141850397664349</v>
       </c>
       <c r="K23">
@@ -3194,7 +3200,7 @@
         <v>21</v>
       </c>
       <c r="M23" s="2">
-        <f>K23/L23*100</f>
+        <f t="shared" si="2"/>
         <v>90.476190476190482</v>
       </c>
     </row>
@@ -3203,7 +3209,7 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <f>E24/30</f>
+        <f t="shared" si="6"/>
         <v>477</v>
       </c>
       <c r="D24">
@@ -3213,22 +3219,22 @@
         <v>14310</v>
       </c>
       <c r="F24" s="2">
-        <f>D24/E24*100</f>
+        <f t="shared" si="7"/>
         <v>5.5206149545772192</v>
       </c>
       <c r="G24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>790</v>
       </c>
       <c r="H24">
         <v>854</v>
       </c>
       <c r="I24" s="2">
-        <f>D24/H24*100</f>
+        <f t="shared" si="0"/>
         <v>92.505854800936774</v>
       </c>
       <c r="J24" s="2">
-        <f>2*F24*I24/(F24+I24)</f>
+        <f t="shared" si="1"/>
         <v>10.419414402532313</v>
       </c>
       <c r="K24">
@@ -3238,7 +3244,7 @@
         <v>16</v>
       </c>
       <c r="M24" s="2">
-        <f>K24/L24*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -3250,7 +3256,7 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <f>E25/30</f>
+        <f t="shared" si="6"/>
         <v>145</v>
       </c>
       <c r="D25">
@@ -3260,22 +3266,22 @@
         <v>4350</v>
       </c>
       <c r="F25" s="2">
-        <f>D25/E25*100</f>
+        <f t="shared" si="7"/>
         <v>74.459770114942529</v>
       </c>
       <c r="G25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3239</v>
       </c>
       <c r="H25">
         <v>6522</v>
       </c>
       <c r="I25" s="2">
-        <f>D25/H25*100</f>
+        <f t="shared" si="0"/>
         <v>49.662680159460287</v>
       </c>
       <c r="J25" s="2">
-        <f>2*F25*I25/(F25+I25)</f>
+        <f t="shared" si="1"/>
         <v>59.58425312729949</v>
       </c>
       <c r="K25">
@@ -3285,7 +3291,7 @@
         <v>32</v>
       </c>
       <c r="M25" s="2">
-        <f>K25/L25*100</f>
+        <f t="shared" si="2"/>
         <v>43.75</v>
       </c>
     </row>
@@ -3294,7 +3300,7 @@
         <v>31</v>
       </c>
       <c r="C26">
-        <f>E26/30</f>
+        <f t="shared" si="6"/>
         <v>177</v>
       </c>
       <c r="D26">
@@ -3304,22 +3310,22 @@
         <v>5310</v>
       </c>
       <c r="F26" s="2">
-        <f>D26/E26*100</f>
+        <f t="shared" si="7"/>
         <v>75.687382297551792</v>
       </c>
       <c r="G26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4019</v>
       </c>
       <c r="H26">
         <v>6940</v>
       </c>
       <c r="I26" s="2">
-        <f>D26/H26*100</f>
+        <f t="shared" si="0"/>
         <v>57.910662824207492</v>
       </c>
       <c r="J26" s="2">
-        <f>2*F26*I26/(F26+I26)</f>
+        <f t="shared" si="1"/>
         <v>65.616326530612241</v>
       </c>
       <c r="K26">
@@ -3329,7 +3335,7 @@
         <v>33</v>
       </c>
       <c r="M26" s="2">
-        <f>K26/L26*100</f>
+        <f t="shared" si="2"/>
         <v>63.636363636363633</v>
       </c>
     </row>
@@ -3338,7 +3344,7 @@
         <v>44</v>
       </c>
       <c r="C27">
-        <f>E27/30</f>
+        <f t="shared" si="6"/>
         <v>157</v>
       </c>
       <c r="D27">
@@ -3348,22 +3354,22 @@
         <v>4710</v>
       </c>
       <c r="F27" s="2">
-        <f>D27/E27*100</f>
+        <f t="shared" si="7"/>
         <v>78.386411889596602</v>
       </c>
       <c r="G27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3692</v>
       </c>
       <c r="H27">
         <v>7092</v>
       </c>
       <c r="I27" s="2">
-        <f>D27/H27*100</f>
+        <f t="shared" si="0"/>
         <v>52.058657642413984</v>
       </c>
       <c r="J27" s="2">
-        <f>2*F27*I27/(F27+I27)</f>
+        <f t="shared" si="1"/>
         <v>62.565666836129459</v>
       </c>
       <c r="K27">
@@ -3373,7 +3379,7 @@
         <v>32</v>
       </c>
       <c r="M27" s="2">
-        <f>K27/L27*100</f>
+        <f t="shared" si="2"/>
         <v>62.5</v>
       </c>
     </row>
@@ -3463,7 +3469,7 @@
         <v>710</v>
       </c>
       <c r="I2" s="2">
-        <f>D2/H2*100</f>
+        <f t="shared" ref="I2:I27" si="0">D2/H2*100</f>
         <v>87.323943661971825</v>
       </c>
       <c r="J2" s="2">
@@ -3486,7 +3492,7 @@
         <v>13</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C29" si="0">E3/30</f>
+        <f t="shared" ref="C3:C20" si="1">E3/30</f>
         <v>181</v>
       </c>
       <c r="D3">
@@ -3496,22 +3502,22 @@
         <v>5430</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F29" si="1">D3/E3*100</f>
+        <f t="shared" ref="F3:F20" si="2">D3/E3*100</f>
         <v>13.425414364640883</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G27" si="2">D3</f>
+        <f t="shared" ref="G3:G27" si="3">D3</f>
         <v>729</v>
       </c>
       <c r="H3">
         <v>809</v>
       </c>
       <c r="I3" s="2">
-        <f>D3/H3*100</f>
+        <f t="shared" si="0"/>
         <v>90.111248454882571</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J27" si="3">2 * F3*I3/(F3+I3)</f>
+        <f t="shared" ref="J3:J27" si="4">2 * F3*I3/(F3+I3)</f>
         <v>23.369129668216061</v>
       </c>
       <c r="K3">
@@ -3521,7 +3527,7 @@
         <v>7</v>
       </c>
       <c r="M3" s="2">
-        <f t="shared" ref="M3:M27" si="4">K3/L3*100</f>
+        <f t="shared" ref="M3:M27" si="5">K3/L3*100</f>
         <v>85.714285714285708</v>
       </c>
     </row>
@@ -3530,7 +3536,7 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>149</v>
       </c>
       <c r="D4">
@@ -3540,22 +3546,22 @@
         <v>4470</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>56.06263982102908</v>
       </c>
       <c r="G4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2506</v>
       </c>
       <c r="H4">
         <v>3873</v>
       </c>
       <c r="I4" s="2">
-        <f>D4/H4*100</f>
+        <f t="shared" si="0"/>
         <v>64.70436354247353</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>60.074313795996638</v>
       </c>
       <c r="K4">
@@ -3565,7 +3571,7 @@
         <v>20</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
     </row>
@@ -3574,7 +3580,7 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="D5">
@@ -3584,22 +3590,22 @@
         <v>1770</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.666666666666667</v>
       </c>
       <c r="G5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>118</v>
       </c>
       <c r="H5">
         <v>136</v>
       </c>
       <c r="I5" s="2">
-        <f>D5/H5*100</f>
+        <f t="shared" si="0"/>
         <v>86.764705882352942</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12.381951731374608</v>
       </c>
       <c r="K5">
@@ -3609,7 +3615,7 @@
         <v>2</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
     </row>
@@ -3618,7 +3624,7 @@
         <v>16</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>139</v>
       </c>
       <c r="D6">
@@ -3628,22 +3634,22 @@
         <v>4170</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31.031175059952037</v>
       </c>
       <c r="G6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1294</v>
       </c>
       <c r="H6">
         <v>1783</v>
       </c>
       <c r="I6" s="2">
-        <f>D6/H6*100</f>
+        <f t="shared" si="0"/>
         <v>72.574312955692648</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43.473878716613477</v>
       </c>
       <c r="K6">
@@ -3653,7 +3659,7 @@
         <v>13</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>84.615384615384613</v>
       </c>
     </row>
@@ -3662,7 +3668,7 @@
         <v>17</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>208</v>
       </c>
       <c r="D7">
@@ -3672,22 +3678,22 @@
         <v>6240</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.5961538461538458</v>
       </c>
       <c r="G7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>474</v>
       </c>
       <c r="H7">
         <v>505</v>
       </c>
       <c r="I7" s="2">
-        <f>D7/H7*100</f>
+        <f t="shared" si="0"/>
         <v>93.861386138613852</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14.054855448480355</v>
       </c>
       <c r="K7">
@@ -3697,7 +3703,7 @@
         <v>6</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
     </row>
@@ -3706,7 +3712,7 @@
         <v>18</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>334</v>
       </c>
       <c r="D8">
@@ -3716,22 +3722,22 @@
         <v>10020</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12974051896207586</v>
       </c>
       <c r="G8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="H8">
         <v>13</v>
       </c>
       <c r="I8" s="2">
-        <f>D8/H8*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.25914482208711254</v>
       </c>
       <c r="K8">
@@ -3741,7 +3747,7 @@
         <v>1</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
     </row>
@@ -3750,7 +3756,7 @@
         <v>19</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>284</v>
       </c>
       <c r="D9">
@@ -3760,22 +3766,22 @@
         <v>8520</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.241784037558686</v>
       </c>
       <c r="G9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1043</v>
       </c>
       <c r="H9">
         <v>1203</v>
       </c>
       <c r="I9" s="2">
-        <f>D9/H9*100</f>
+        <f t="shared" si="0"/>
         <v>86.699916874480465</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21.454283657307414</v>
       </c>
       <c r="K9">
@@ -3785,7 +3791,7 @@
         <v>3</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
     </row>
@@ -3794,7 +3800,7 @@
         <v>20</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>285</v>
       </c>
       <c r="D10">
@@ -3804,22 +3810,22 @@
         <v>8550</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.327485380116959</v>
       </c>
       <c r="G10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>199</v>
       </c>
       <c r="H10">
         <v>199</v>
       </c>
       <c r="I10" s="2">
-        <f>D10/H10*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.5490913247228253</v>
       </c>
       <c r="K10">
@@ -3829,7 +3835,7 @@
         <v>2</v>
       </c>
       <c r="M10" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
     </row>
@@ -3838,7 +3844,7 @@
         <v>21</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>337</v>
       </c>
       <c r="D11">
@@ -3848,22 +3854,22 @@
         <v>10110</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.827893175074186</v>
       </c>
       <c r="G11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1398</v>
       </c>
       <c r="H11">
         <v>1913</v>
       </c>
       <c r="I11" s="2">
-        <f>D11/H11*100</f>
+        <f t="shared" si="0"/>
         <v>73.078933612127557</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23.255427098062054</v>
       </c>
       <c r="K11">
@@ -3873,7 +3879,7 @@
         <v>2</v>
       </c>
       <c r="M11" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
     </row>
@@ -3882,7 +3888,7 @@
         <v>22</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>223</v>
       </c>
       <c r="D12">
@@ -3892,22 +3898,22 @@
         <v>6690</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32.765321375186844</v>
       </c>
       <c r="G12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2192</v>
       </c>
       <c r="H12">
         <v>2608</v>
       </c>
       <c r="I12" s="2">
-        <f>D12/H12*100</f>
+        <f t="shared" si="0"/>
         <v>84.049079754601223</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>47.149924714992466</v>
       </c>
       <c r="K12">
@@ -3917,7 +3923,7 @@
         <v>3</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
     </row>
@@ -3926,7 +3932,7 @@
         <v>23</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="D13">
@@ -3936,22 +3942,22 @@
         <v>1410</v>
       </c>
       <c r="F13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>97.872340425531917</v>
       </c>
       <c r="G13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1380</v>
       </c>
       <c r="H13">
         <v>8142</v>
       </c>
       <c r="I13" s="2">
-        <f>D13/H13*100</f>
+        <f t="shared" si="0"/>
         <v>16.949152542372879</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>28.894472361809044</v>
       </c>
       <c r="K13">
@@ -3961,7 +3967,7 @@
         <v>13</v>
       </c>
       <c r="M13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>15.384615384615385</v>
       </c>
     </row>
@@ -3970,7 +3976,7 @@
         <v>24</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>171</v>
       </c>
       <c r="D14">
@@ -3980,22 +3986,22 @@
         <v>5130</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>61.189083820662773</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3139</v>
       </c>
       <c r="H14">
         <v>4532</v>
       </c>
       <c r="I14" s="2">
-        <f>D14/H14*100</f>
+        <f t="shared" si="0"/>
         <v>69.263018534863193</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>64.976195404678123</v>
       </c>
       <c r="K14">
@@ -4005,7 +4011,7 @@
         <v>16</v>
       </c>
       <c r="M14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>62.5</v>
       </c>
     </row>
@@ -4014,7 +4020,7 @@
         <v>25</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>294</v>
       </c>
       <c r="D15">
@@ -4024,22 +4030,22 @@
         <v>8820</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15" s="2" t="e">
-        <f>D15/H15*100</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J15" s="2" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K15">
@@ -4049,7 +4055,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="2" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4058,7 +4064,7 @@
         <v>26</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="D16">
@@ -4068,22 +4074,22 @@
         <v>1320</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>71.893939393939405</v>
       </c>
       <c r="G16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>949</v>
       </c>
       <c r="H16">
         <v>1718</v>
       </c>
       <c r="I16" s="2">
-        <f>D16/H16*100</f>
+        <f t="shared" si="0"/>
         <v>55.238649592549471</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>62.475312705727454</v>
       </c>
       <c r="K16">
@@ -4093,7 +4099,7 @@
         <v>10</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
     </row>
@@ -4102,7 +4108,7 @@
         <v>27</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="D17">
@@ -4112,22 +4118,22 @@
         <v>1170</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="G17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>936</v>
       </c>
       <c r="H17">
         <v>1978</v>
       </c>
       <c r="I17" s="2">
-        <f>D17/H17*100</f>
+        <f t="shared" si="0"/>
         <v>47.320525783619814</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>59.466327827191868</v>
       </c>
       <c r="K17">
@@ -4137,7 +4143,7 @@
         <v>9</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44.444444444444443</v>
       </c>
     </row>
@@ -4146,7 +4152,7 @@
         <v>28</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>116</v>
       </c>
       <c r="D18">
@@ -4156,22 +4162,22 @@
         <v>3480</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39.166666666666664</v>
       </c>
       <c r="G18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1363</v>
       </c>
       <c r="H18">
         <v>1778</v>
       </c>
       <c r="I18" s="2">
-        <f>D18/H18*100</f>
+        <f t="shared" si="0"/>
         <v>76.6591676040495</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>51.844807911753513</v>
       </c>
       <c r="K18">
@@ -4181,7 +4187,7 @@
         <v>14</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>92.857142857142861</v>
       </c>
     </row>
@@ -4190,7 +4196,7 @@
         <v>29</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>128</v>
       </c>
       <c r="D19">
@@ -4200,22 +4206,22 @@
         <v>3840</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60.390625</v>
       </c>
       <c r="G19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2319</v>
       </c>
       <c r="H19">
         <v>3103</v>
       </c>
       <c r="I19" s="2">
-        <f>D19/H19*100</f>
+        <f t="shared" si="0"/>
         <v>74.734128262971325</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>66.801094627682559</v>
       </c>
       <c r="K19">
@@ -4225,7 +4231,7 @@
         <v>14</v>
       </c>
       <c r="M19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>85.714285714285708</v>
       </c>
     </row>
@@ -4234,7 +4240,7 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>74</v>
       </c>
       <c r="D20">
@@ -4244,22 +4250,22 @@
         <v>2220</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18.918918918918919</v>
       </c>
       <c r="G20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>420</v>
       </c>
       <c r="H20">
         <v>463</v>
       </c>
       <c r="I20" s="2">
-        <f>D20/H20*100</f>
+        <f t="shared" si="0"/>
         <v>90.712742980561558</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>31.308237048080507</v>
       </c>
       <c r="K20">
@@ -4269,7 +4275,7 @@
         <v>4</v>
       </c>
       <c r="M20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
     </row>
@@ -4281,7 +4287,7 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <f>E21/30</f>
+        <f t="shared" ref="C21:C27" si="6">E21/30</f>
         <v>259</v>
       </c>
       <c r="D21">
@@ -4291,22 +4297,22 @@
         <v>7770</v>
       </c>
       <c r="F21" s="2">
-        <f>D21/E21*100</f>
+        <f t="shared" ref="F21:F27" si="7">D21/E21*100</f>
         <v>21.557271557271555</v>
       </c>
       <c r="G21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1675</v>
       </c>
       <c r="H21">
         <v>2314</v>
       </c>
       <c r="I21" s="2">
-        <f>D21/H21*100</f>
+        <f t="shared" si="0"/>
         <v>72.385479688850467</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33.220944069813562</v>
       </c>
       <c r="K21">
@@ -4316,7 +4322,7 @@
         <v>25</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>76</v>
       </c>
     </row>
@@ -4325,7 +4331,7 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <f>E22/30</f>
+        <f t="shared" si="6"/>
         <v>91</v>
       </c>
       <c r="D22">
@@ -4335,22 +4341,22 @@
         <v>2730</v>
       </c>
       <c r="F22" s="2">
-        <f>D22/E22*100</f>
+        <f t="shared" si="7"/>
         <v>44.798534798534803</v>
       </c>
       <c r="G22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1223</v>
       </c>
       <c r="H22">
         <v>2383</v>
       </c>
       <c r="I22" s="2">
-        <f>D22/H22*100</f>
+        <f t="shared" si="0"/>
         <v>51.321863197650018</v>
       </c>
       <c r="J22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>47.838842167025227</v>
       </c>
       <c r="K22">
@@ -4360,7 +4366,7 @@
         <v>20</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
     </row>
@@ -4369,7 +4375,7 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <f>E23/30</f>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="D23">
@@ -4379,22 +4385,22 @@
         <v>4500</v>
       </c>
       <c r="F23" s="2">
-        <f>D23/E23*100</f>
+        <f t="shared" si="7"/>
         <v>24.022222222222222</v>
       </c>
       <c r="G23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1081</v>
       </c>
       <c r="H23">
         <v>1683</v>
       </c>
       <c r="I23" s="2">
-        <f>D23/H23*100</f>
+        <f t="shared" si="0"/>
         <v>64.23054070112893</v>
       </c>
       <c r="J23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>34.966844573831473</v>
       </c>
       <c r="K23">
@@ -4404,7 +4410,7 @@
         <v>21</v>
       </c>
       <c r="M23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>76.19047619047619</v>
       </c>
     </row>
@@ -4413,7 +4419,7 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <f>E24/30</f>
+        <f t="shared" si="6"/>
         <v>387</v>
       </c>
       <c r="D24">
@@ -4423,22 +4429,22 @@
         <v>11610</v>
       </c>
       <c r="F24" s="2">
-        <f>D24/E24*100</f>
+        <f t="shared" si="7"/>
         <v>6.416881998277348</v>
       </c>
       <c r="G24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>745</v>
       </c>
       <c r="H24">
         <v>854</v>
       </c>
       <c r="I24" s="2">
-        <f>D24/H24*100</f>
+        <f t="shared" si="0"/>
         <v>87.236533957845424</v>
       </c>
       <c r="J24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.954428754813865</v>
       </c>
       <c r="K24">
@@ -4448,7 +4454,7 @@
         <v>16</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>87.5</v>
       </c>
     </row>
@@ -4460,7 +4466,7 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <f>E25/30</f>
+        <f t="shared" si="6"/>
         <v>94</v>
       </c>
       <c r="D25">
@@ -4470,22 +4476,22 @@
         <v>2820</v>
       </c>
       <c r="F25" s="2">
-        <f>D25/E25*100</f>
+        <f t="shared" si="7"/>
         <v>83.652482269503551</v>
       </c>
       <c r="G25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2359</v>
       </c>
       <c r="H25">
         <v>6522</v>
       </c>
       <c r="I25" s="2">
-        <f>D25/H25*100</f>
+        <f t="shared" si="0"/>
         <v>36.169886537871818</v>
       </c>
       <c r="J25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50.503104260329692</v>
       </c>
       <c r="K25">
@@ -4495,7 +4501,7 @@
         <v>32</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
     </row>
@@ -4504,7 +4510,7 @@
         <v>31</v>
       </c>
       <c r="C26">
-        <f>E26/30</f>
+        <f t="shared" si="6"/>
         <v>108</v>
       </c>
       <c r="D26">
@@ -4514,22 +4520,22 @@
         <v>3240</v>
       </c>
       <c r="F26" s="2">
-        <f>D26/E26*100</f>
+        <f t="shared" si="7"/>
         <v>84.938271604938279</v>
       </c>
       <c r="G26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2752</v>
       </c>
       <c r="H26">
         <v>6940</v>
       </c>
       <c r="I26" s="2">
-        <f>D26/H26*100</f>
+        <f t="shared" si="0"/>
         <v>39.654178674351584</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>54.06679764243615</v>
       </c>
       <c r="K26">
@@ -4539,7 +4545,7 @@
         <v>33</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>36.363636363636367</v>
       </c>
     </row>
@@ -4548,7 +4554,7 @@
         <v>44</v>
       </c>
       <c r="C27">
-        <f>E27/30</f>
+        <f t="shared" si="6"/>
         <v>89</v>
       </c>
       <c r="D27">
@@ -4558,22 +4564,22 @@
         <v>2670</v>
       </c>
       <c r="F27" s="2">
-        <f>D27/E27*100</f>
+        <f t="shared" si="7"/>
         <v>77.677902621722851</v>
       </c>
       <c r="G27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2074</v>
       </c>
       <c r="H27">
         <v>7092</v>
       </c>
       <c r="I27" s="2">
-        <f>D27/H27*100</f>
+        <f t="shared" si="0"/>
         <v>29.244218838127466</v>
       </c>
       <c r="J27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>42.491292767875436</v>
       </c>
       <c r="K27">
@@ -4583,7 +4589,7 @@
         <v>32</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
     </row>
@@ -4673,7 +4679,7 @@
         <v>710</v>
       </c>
       <c r="I2" s="2">
-        <f>D2/H2*100</f>
+        <f t="shared" ref="I2:I27" si="0">D2/H2*100</f>
         <v>46.760563380281688</v>
       </c>
       <c r="J2" s="2">
@@ -4696,7 +4702,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C20" si="0">E3/30</f>
+        <f t="shared" ref="C3:C20" si="1">E3/30</f>
         <v>36.666666666666664</v>
       </c>
       <c r="D3">
@@ -4706,22 +4712,22 @@
         <v>1100</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F20" si="1">D3/E3*100</f>
+        <f t="shared" ref="F3:F20" si="2">D3/E3*100</f>
         <v>28.636363636363637</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G27" si="2">D3</f>
+        <f t="shared" ref="G3:G27" si="3">D3</f>
         <v>315</v>
       </c>
       <c r="H3">
         <v>809</v>
       </c>
       <c r="I3" s="2">
-        <f>D3/H3*100</f>
+        <f t="shared" si="0"/>
         <v>38.936959208899871</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J27" si="3">2*F3*I3/(F3+I3)</f>
+        <f t="shared" ref="J3:J27" si="4">2*F3*I3/(F3+I3)</f>
         <v>33.001571503404925</v>
       </c>
       <c r="K3">
@@ -4731,7 +4737,7 @@
         <v>7</v>
       </c>
       <c r="M3" s="2">
-        <f t="shared" ref="M3:M27" si="4">K3/L3*100</f>
+        <f t="shared" ref="M3:M27" si="5">K3/L3*100</f>
         <v>28.571428571428569</v>
       </c>
     </row>
@@ -4740,7 +4746,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>215</v>
       </c>
       <c r="D4">
@@ -4750,22 +4756,22 @@
         <v>6450</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.100775193798452</v>
       </c>
       <c r="G4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1877</v>
       </c>
       <c r="H4">
         <v>3873</v>
       </c>
       <c r="I4" s="2">
-        <f>D4/H4*100</f>
+        <f t="shared" si="0"/>
         <v>48.463723211980373</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.365397655720237</v>
       </c>
       <c r="K4">
@@ -4775,7 +4781,7 @@
         <v>20</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
     </row>
@@ -4784,7 +4790,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.0333333333333332</v>
       </c>
       <c r="D5">
@@ -4794,22 +4800,22 @@
         <v>151</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>61.589403973509938</v>
       </c>
       <c r="G5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>93</v>
       </c>
       <c r="H5">
         <v>136</v>
       </c>
       <c r="I5" s="2">
-        <f>D5/H5*100</f>
+        <f t="shared" si="0"/>
         <v>68.382352941176478</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>64.808362369337985</v>
       </c>
       <c r="K5">
@@ -4819,7 +4825,7 @@
         <v>2</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
     </row>
@@ -4828,7 +4834,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="D6">
@@ -4838,22 +4844,22 @@
         <v>1500</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53.533333333333331</v>
       </c>
       <c r="G6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>803</v>
       </c>
       <c r="H6">
         <v>1783</v>
       </c>
       <c r="I6" s="2">
-        <f>D6/H6*100</f>
+        <f t="shared" si="0"/>
         <v>45.036455412226587</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>48.918671946390496</v>
       </c>
       <c r="K6">
@@ -4863,7 +4869,7 @@
         <v>13</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30.76923076923077</v>
       </c>
     </row>
@@ -4872,7 +4878,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41.666666666666664</v>
       </c>
       <c r="D7">
@@ -4882,22 +4888,22 @@
         <v>1250</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19.52</v>
       </c>
       <c r="G7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>244</v>
       </c>
       <c r="H7">
         <v>505</v>
       </c>
       <c r="I7" s="2">
-        <f>D7/H7*100</f>
+        <f t="shared" si="0"/>
         <v>48.316831683168317</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27.806267806267805</v>
       </c>
       <c r="K7">
@@ -4907,7 +4913,7 @@
         <v>6</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>66.666666666666657</v>
       </c>
     </row>
@@ -4916,7 +4922,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="D8">
@@ -4926,22 +4932,22 @@
         <v>50</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H8">
         <v>13</v>
       </c>
       <c r="I8" s="2">
-        <f>D8/H8*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J8" s="2" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K8">
@@ -4951,7 +4957,7 @@
         <v>1</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4960,7 +4966,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="D9">
@@ -4970,22 +4976,22 @@
         <v>600</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91.666666666666657</v>
       </c>
       <c r="G9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>550</v>
       </c>
       <c r="H9">
         <v>1203</v>
       </c>
       <c r="I9" s="2">
-        <f>D9/H9*100</f>
+        <f t="shared" si="0"/>
         <v>45.7190357439734</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>61.009428729894623</v>
       </c>
       <c r="K9">
@@ -4995,7 +5001,7 @@
         <v>3</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5004,7 +5010,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="D10">
@@ -5014,22 +5020,22 @@
         <v>100</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="G10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="H10">
         <v>199</v>
       </c>
       <c r="I10" s="2">
-        <f>D10/H10*100</f>
+        <f t="shared" si="0"/>
         <v>25.125628140703515</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33.444816053511708</v>
       </c>
       <c r="K10">
@@ -5039,7 +5045,7 @@
         <v>2</v>
       </c>
       <c r="M10" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5048,7 +5054,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="D11">
@@ -5058,22 +5064,22 @@
         <v>600</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91.666666666666657</v>
       </c>
       <c r="G11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>550</v>
       </c>
       <c r="H11">
         <v>1913</v>
       </c>
       <c r="I11" s="2">
-        <f>D11/H11*100</f>
+        <f t="shared" si="0"/>
         <v>28.750653423941451</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43.772383605252678</v>
       </c>
       <c r="K11">
@@ -5083,7 +5089,7 @@
         <v>2</v>
       </c>
       <c r="M11" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5092,7 +5098,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28.333333333333332</v>
       </c>
       <c r="D12">
@@ -5102,22 +5108,22 @@
         <v>850</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>94.117647058823522</v>
       </c>
       <c r="G12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>800</v>
       </c>
       <c r="H12">
         <v>2608</v>
       </c>
       <c r="I12" s="2">
-        <f>D12/H12*100</f>
+        <f t="shared" si="0"/>
         <v>30.674846625766872</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>46.26951995373048</v>
       </c>
       <c r="K12">
@@ -5127,7 +5133,7 @@
         <v>3</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5136,7 +5142,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>163.33333333333334</v>
       </c>
       <c r="D13">
@@ -5146,22 +5152,22 @@
         <v>4900</v>
       </c>
       <c r="F13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>62.469387755102048</v>
       </c>
       <c r="G13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3061</v>
       </c>
       <c r="H13">
         <v>8142</v>
       </c>
       <c r="I13" s="2">
-        <f>D13/H13*100</f>
+        <f t="shared" si="0"/>
         <v>37.595185458118394</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>46.940653274037722</v>
       </c>
       <c r="K13">
@@ -5171,7 +5177,7 @@
         <v>13</v>
       </c>
       <c r="M13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23.076923076923077</v>
       </c>
     </row>
@@ -5180,7 +5186,7 @@
         <v>24</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>215</v>
       </c>
       <c r="D14">
@@ -5190,22 +5196,22 @@
         <v>6450</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35.193798449612402</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2270</v>
       </c>
       <c r="H14">
         <v>4532</v>
       </c>
       <c r="I14" s="2">
-        <f>D14/H14*100</f>
+        <f t="shared" si="0"/>
         <v>50.088261253309796</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>41.340375159351666</v>
       </c>
       <c r="K14">
@@ -5215,7 +5221,7 @@
         <v>16</v>
       </c>
       <c r="M14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>37.5</v>
       </c>
     </row>
@@ -5224,7 +5230,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>213.33333333333334</v>
       </c>
       <c r="D15">
@@ -5234,22 +5240,22 @@
         <v>6400</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15" s="2" t="e">
-        <f>D15/H15*100</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J15" s="2" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K15">
@@ -5259,7 +5265,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="2" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -5268,7 +5274,7 @@
         <v>26</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.366666666666667</v>
       </c>
       <c r="D16">
@@ -5278,22 +5284,22 @@
         <v>671</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>78.539493293591661</v>
       </c>
       <c r="G16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>527</v>
       </c>
       <c r="H16">
         <v>1718</v>
       </c>
       <c r="I16" s="2">
-        <f>D16/H16*100</f>
+        <f t="shared" si="0"/>
         <v>30.675203725261934</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>44.118878191712014</v>
       </c>
       <c r="K16">
@@ -5303,7 +5309,7 @@
         <v>10</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
@@ -5312,7 +5318,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23.333333333333332</v>
       </c>
       <c r="D17">
@@ -5322,22 +5328,22 @@
         <v>700</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91</v>
       </c>
       <c r="G17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>637</v>
       </c>
       <c r="H17">
         <v>1978</v>
       </c>
       <c r="I17" s="2">
-        <f>D17/H17*100</f>
+        <f t="shared" si="0"/>
         <v>32.204246713852378</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>47.572815533980588</v>
       </c>
       <c r="K17">
@@ -5347,7 +5353,7 @@
         <v>9</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11.111111111111111</v>
       </c>
     </row>
@@ -5356,7 +5362,7 @@
         <v>28</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="D18">
@@ -5366,22 +5372,22 @@
         <v>1350</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64.222222222222229</v>
       </c>
       <c r="G18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>867</v>
       </c>
       <c r="H18">
         <v>1778</v>
       </c>
       <c r="I18" s="2">
-        <f>D18/H18*100</f>
+        <f t="shared" si="0"/>
         <v>48.762654668166476</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>55.434782608695649</v>
       </c>
       <c r="K18">
@@ -5391,7 +5397,7 @@
         <v>14</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>57.142857142857139</v>
       </c>
     </row>
@@ -5400,7 +5406,7 @@
         <v>29</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>210</v>
       </c>
       <c r="D19">
@@ -5410,22 +5416,22 @@
         <v>6300</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24.174603174603174</v>
       </c>
       <c r="G19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1523</v>
       </c>
       <c r="H19">
         <v>3103</v>
       </c>
       <c r="I19" s="2">
-        <f>D19/H19*100</f>
+        <f t="shared" si="0"/>
         <v>49.081533999355464</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32.393916835052643</v>
       </c>
       <c r="K19">
@@ -5435,7 +5441,7 @@
         <v>14</v>
       </c>
       <c r="M19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>57.142857142857139</v>
       </c>
     </row>
@@ -5444,7 +5450,7 @@
         <v>38</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21.666666666666668</v>
       </c>
       <c r="D20">
@@ -5454,22 +5460,22 @@
         <v>650</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.076923076923077</v>
       </c>
       <c r="G20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>189</v>
       </c>
       <c r="H20">
         <v>463</v>
       </c>
       <c r="I20" s="2">
-        <f>D20/H20*100</f>
+        <f t="shared" si="0"/>
         <v>40.820734341252702</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33.96226415094339</v>
       </c>
       <c r="K20">
@@ -5479,7 +5485,7 @@
         <v>4</v>
       </c>
       <c r="M20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5491,7 +5497,7 @@
         <v>39</v>
       </c>
       <c r="C21" s="1">
-        <f>E21/30</f>
+        <f t="shared" ref="C21:C27" si="6">E21/30</f>
         <v>165</v>
       </c>
       <c r="D21">
@@ -5501,22 +5507,22 @@
         <v>4950</v>
       </c>
       <c r="F21" s="2">
-        <f>D21/E21*100</f>
+        <f t="shared" ref="F21:F27" si="7">D21/E21*100</f>
         <v>22.525252525252526</v>
       </c>
       <c r="G21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1115</v>
       </c>
       <c r="H21">
         <v>2314</v>
       </c>
       <c r="I21" s="2">
-        <f>D21/H21*100</f>
+        <f t="shared" si="0"/>
         <v>48.184961106309423</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>30.699339207048464</v>
       </c>
       <c r="K21">
@@ -5526,7 +5532,7 @@
         <v>25</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44</v>
       </c>
     </row>
@@ -5535,7 +5541,7 @@
         <v>40</v>
       </c>
       <c r="C22" s="1">
-        <f>E22/30</f>
+        <f t="shared" si="6"/>
         <v>232.6</v>
       </c>
       <c r="D22">
@@ -5545,22 +5551,22 @@
         <v>6978</v>
       </c>
       <c r="F22" s="2">
-        <f>D22/E22*100</f>
+        <f t="shared" si="7"/>
         <v>17.282889079965607</v>
       </c>
       <c r="G22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1206</v>
       </c>
       <c r="H22">
         <v>2383</v>
       </c>
       <c r="I22" s="2">
-        <f>D22/H22*100</f>
+        <f t="shared" si="0"/>
         <v>50.608476710029372</v>
       </c>
       <c r="J22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25.766477940390985</v>
       </c>
       <c r="K22">
@@ -5570,7 +5576,7 @@
         <v>20</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
     </row>
@@ -5579,7 +5585,7 @@
         <v>41</v>
       </c>
       <c r="C23" s="1">
-        <f>E23/30</f>
+        <f t="shared" si="6"/>
         <v>227.06666666666666</v>
       </c>
       <c r="D23">
@@ -5589,22 +5595,22 @@
         <v>6812</v>
       </c>
       <c r="F23" s="2">
-        <f>D23/E23*100</f>
+        <f t="shared" si="7"/>
         <v>11.890780974750442</v>
       </c>
       <c r="G23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>810</v>
       </c>
       <c r="H23">
         <v>1683</v>
       </c>
       <c r="I23" s="2">
-        <f>D23/H23*100</f>
+        <f t="shared" si="0"/>
         <v>48.128342245989302</v>
       </c>
       <c r="J23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19.070041200706299</v>
       </c>
       <c r="K23">
@@ -5614,7 +5620,7 @@
         <v>21</v>
       </c>
       <c r="M23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>33.333333333333329</v>
       </c>
     </row>
@@ -5623,7 +5629,7 @@
         <v>42</v>
       </c>
       <c r="C24" s="1">
-        <f>E24/30</f>
+        <f t="shared" si="6"/>
         <v>231.6</v>
       </c>
       <c r="D24">
@@ -5633,22 +5639,22 @@
         <v>6948</v>
       </c>
       <c r="F24" s="2">
-        <f>D24/E24*100</f>
+        <f t="shared" si="7"/>
         <v>5.8146229130685088</v>
       </c>
       <c r="G24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>404</v>
       </c>
       <c r="H24">
         <v>854</v>
       </c>
       <c r="I24" s="2">
-        <f>D24/H24*100</f>
+        <f t="shared" si="0"/>
         <v>47.306791569086656</v>
       </c>
       <c r="J24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10.356318892591641</v>
       </c>
       <c r="K24">
@@ -5658,7 +5664,7 @@
         <v>16</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>56.25</v>
       </c>
     </row>
@@ -5670,7 +5676,7 @@
         <v>43</v>
       </c>
       <c r="C25" s="1">
-        <f>E25/30</f>
+        <f t="shared" si="6"/>
         <v>249.46666666666667</v>
       </c>
       <c r="D25">
@@ -5680,22 +5686,22 @@
         <v>7484</v>
       </c>
       <c r="F25" s="2">
-        <f>D25/E25*100</f>
+        <f t="shared" si="7"/>
         <v>43.586317477284872</v>
       </c>
       <c r="G25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3262</v>
       </c>
       <c r="H25">
         <v>6522</v>
       </c>
       <c r="I25" s="2">
-        <f>D25/H25*100</f>
+        <f t="shared" si="0"/>
         <v>50.015332720024531</v>
       </c>
       <c r="J25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>46.580037126945598</v>
       </c>
       <c r="K25">
@@ -5705,7 +5711,7 @@
         <v>32</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>40.625</v>
       </c>
     </row>
@@ -5714,7 +5720,7 @@
         <v>31</v>
       </c>
       <c r="C26" s="1">
-        <f>E26/30</f>
+        <f t="shared" si="6"/>
         <v>247.36666666666667</v>
       </c>
       <c r="D26">
@@ -5724,22 +5730,22 @@
         <v>7421</v>
       </c>
       <c r="F26" s="2">
-        <f>D26/E26*100</f>
+        <f t="shared" si="7"/>
         <v>46.947850693976548</v>
       </c>
       <c r="G26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3484</v>
       </c>
       <c r="H26">
         <v>6940</v>
       </c>
       <c r="I26" s="2">
-        <f>D26/H26*100</f>
+        <f t="shared" si="0"/>
         <v>50.201729106628243</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>48.520298029385138</v>
       </c>
       <c r="K26">
@@ -5749,7 +5755,7 @@
         <v>33</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>54.54545454545454</v>
       </c>
     </row>
@@ -5758,7 +5764,7 @@
         <v>44</v>
       </c>
       <c r="C27" s="1">
-        <f>E27/30</f>
+        <f t="shared" si="6"/>
         <v>247.7</v>
       </c>
       <c r="D27">
@@ -5768,22 +5774,22 @@
         <v>7431</v>
       </c>
       <c r="F27" s="2">
-        <f>D27/E27*100</f>
+        <f t="shared" si="7"/>
         <v>48.055443412730455</v>
       </c>
       <c r="G27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3571</v>
       </c>
       <c r="H27">
         <v>7092</v>
       </c>
       <c r="I27" s="2">
-        <f>D27/H27*100</f>
+        <f t="shared" si="0"/>
         <v>50.352509870276364</v>
       </c>
       <c r="J27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>49.177167251945185</v>
       </c>
       <c r="K27">
@@ -5793,7 +5799,7 @@
         <v>32</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>53.125</v>
       </c>
     </row>

</xml_diff>